<commit_message>
Correcciones en el dashboard
</commit_message>
<xml_diff>
--- a/Dashboards/Data final/brechas_salariales.xlsx
+++ b/Dashboards/Data final/brechas_salariales.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -388,7 +388,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>318.9621412807595</v>
+        <v>1174.327812754051</v>
       </c>
     </row>
     <row r="3">
@@ -397,11 +397,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Secundaria</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C3">
-        <v>11.18786982248521</v>
+        <v>184.54637756707</v>
       </c>
     </row>
     <row r="4">
@@ -410,24 +410,24 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C4">
-        <v>27.98603351955307</v>
+        <v>298.0739908525634</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="C5">
-        <v>332.1259141618897</v>
+        <v>633.7139923384145</v>
       </c>
     </row>
     <row r="6">
@@ -436,50 +436,50 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Posgrado</t>
         </is>
       </c>
       <c r="C6">
-        <v>48.17350157728707</v>
+        <v>1092.069452558507</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C7">
-        <v>323.3883076433889</v>
+        <v>200.3236529360932</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Primaria/Básica</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C8">
-        <v>84.95135135135135</v>
+        <v>327.164275027676</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Secundaria</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="C9">
-        <v>33.67018469656992</v>
+        <v>603.7327752509223</v>
       </c>
     </row>
     <row r="10">
@@ -488,42 +488,42 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Posgrado</t>
         </is>
       </c>
       <c r="C10">
-        <v>22.07435897435898</v>
+        <v>1339.195741447326</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C11">
-        <v>364.5535457665391</v>
+        <v>206.5929174545637</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C12">
-        <v>384.3845465331659</v>
+        <v>310.498371345067</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -531,12 +531,12 @@
         </is>
       </c>
       <c r="C13">
-        <v>17</v>
+        <v>564.5614243552058</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -544,90 +544,90 @@
         </is>
       </c>
       <c r="C14">
-        <v>422.0752106390173</v>
+        <v>1181.975518762201</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>229.2629523856647</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C16">
-        <v>469.3868293358107</v>
+        <v>329.7101527053014</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Secundaria</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>650.8579000717997</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Posgrado</t>
         </is>
       </c>
       <c r="C18">
-        <v>70</v>
+        <v>1179.80566018528</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C19">
-        <v>486.6780976954748</v>
+        <v>247.4960441630431</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C20">
-        <v>512.7847208895593</v>
+        <v>377.2134090536833</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>2015</v>
+        <v>2011</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -635,12 +635,12 @@
         </is>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>635.0909405131441</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -648,38 +648,38 @@
         </is>
       </c>
       <c r="C22">
-        <v>489.695647136462</v>
+        <v>1305.869432801143</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Superior</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>270.3323487875374</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C24">
-        <v>494.1259524882821</v>
+        <v>415.1937716334246</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -687,12 +687,12 @@
         </is>
       </c>
       <c r="C25">
-        <v>96.31807228915663</v>
+        <v>681.4452164826836</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -700,51 +700,51 @@
         </is>
       </c>
       <c r="C26">
-        <v>483.3833628542529</v>
+        <v>1758.278173669468</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Secundaria</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C27">
-        <v>100</v>
+        <v>283.9019785229411</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C28">
-        <v>472.1362615671298</v>
+        <v>424.3308704043537</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>2020</v>
+        <v>2013</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Superior</t>
         </is>
       </c>
       <c r="C29">
-        <v>424.526403628908</v>
+        <v>817.5091677302175</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>2021</v>
+        <v>2014</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -752,46 +752,566 @@
         </is>
       </c>
       <c r="C30">
-        <v>438.5705964772461</v>
+        <v>1717.764837639251</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>2022</v>
+        <v>2014</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Primaria/Básica</t>
         </is>
       </c>
       <c r="C31">
-        <v>471.3764140181302</v>
+        <v>320.1463634417079</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>2023</v>
+        <v>2014</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Posgrado</t>
+          <t>Secundaria</t>
         </is>
       </c>
       <c r="C32">
-        <v>460.6123741655142</v>
+        <v>451.9342169749407</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
+        <v>2014</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>815.0458243442184</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>2015</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>1863.332933261013</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2015</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>329.2948994700325</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2015</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>459.6701340400256</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>2015</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>855.3722129104153</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>2016</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>1647.459228461368</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>2016</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>314.2216087192808</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>2016</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>437.6311629384669</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>2016</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>826.486746077515</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>2017</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>1620.457104606144</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>2017</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>322.1999178440681</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>2017</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>452.9415150428886</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>2017</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>798.8045434942279</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>2018</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>1703.329609388277</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>2018</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>310.5684118995</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2018</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>440.1729804592302</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>2018</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>800.1295367162019</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>2019</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>1564.478500709603</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>302.8906803255705</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>2019</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>432.5607419980601</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2019</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>775.9403457467339</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2020</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>1471.117804781876</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>2020</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>263.0168088047251</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>2020</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C56">
+        <v>368.5476354368428</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>2020</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C57">
+        <v>748.6741843396296</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>2021</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C58">
+        <v>1645.123571056422</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>2021</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C59">
+        <v>266.8814033820425</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>2021</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C60">
+        <v>386.1955911630345</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>2021</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C61">
+        <v>707.6446436056895</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>2022</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C62">
+        <v>1500.441437920619</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>2022</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C63">
+        <v>296.5247730235982</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>2022</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C64">
+        <v>419.4798019941964</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>2022</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C65">
+        <v>752.6673844149784</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>2023</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Posgrado</t>
+        </is>
+      </c>
+      <c r="C66">
+        <v>1375.667855540071</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>2023</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C67">
+        <v>308.9442935911447</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>2023</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>417.5949046319496</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>2023</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C69">
+        <v>705.1020256982231</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
         <v>2024</v>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>Posgrado</t>
         </is>
       </c>
-      <c r="C33">
-        <v>447.2688240083684</v>
+      <c r="C70">
+        <v>1369.091332931051</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>2024</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Primaria/Básica</t>
+        </is>
+      </c>
+      <c r="C71">
+        <v>288.8791543489164</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>2024</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Secundaria</t>
+        </is>
+      </c>
+      <c r="C72">
+        <v>433.849530384189</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>2024</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>Superior</t>
+        </is>
+      </c>
+      <c r="C73">
+        <v>691.3764448484419</v>
       </c>
     </row>
   </sheetData>
@@ -801,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -834,7 +1354,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>384.7473789252037</v>
+        <v>353.2451775611751</v>
       </c>
     </row>
     <row r="3">
@@ -847,7 +1367,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>244.7986769602632</v>
+        <v>257.021343823485</v>
       </c>
     </row>
     <row r="4">
@@ -860,7 +1380,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>394.3527417949346</v>
+        <v>363.7197767863112</v>
       </c>
     </row>
     <row r="5">
@@ -873,7 +1393,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>264.1963036597876</v>
+        <v>276.049152753157</v>
       </c>
     </row>
     <row r="6">
@@ -886,7 +1406,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>377.0032532398213</v>
+        <v>351.6280513061309</v>
       </c>
     </row>
     <row r="7">
@@ -899,7 +1419,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>266.5490683215139</v>
+        <v>273.6590362067911</v>
       </c>
     </row>
     <row r="8">
@@ -912,7 +1432,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>417.4777047274521</v>
+        <v>389.1969402627565</v>
       </c>
     </row>
     <row r="9">
@@ -925,7 +1445,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>309.6056567269835</v>
+        <v>319.9352434078944</v>
       </c>
     </row>
     <row r="10">
@@ -938,7 +1458,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>424.634390324853</v>
+        <v>413.5236522160682</v>
       </c>
     </row>
     <row r="11">
@@ -951,7 +1471,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>338.941434883193</v>
+        <v>332.0452706286642</v>
       </c>
     </row>
     <row r="12">
@@ -964,7 +1484,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>455.5822220279414</v>
+        <v>448.5792615853337</v>
       </c>
     </row>
     <row r="13">
@@ -977,7 +1497,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>386.3716144129093</v>
+        <v>375.649527714834</v>
       </c>
     </row>
     <row r="14">
@@ -990,7 +1510,7 @@
         </is>
       </c>
       <c r="C14">
-        <v>519.0921207802531</v>
+        <v>507.3238221337621</v>
       </c>
     </row>
     <row r="15">
@@ -1003,7 +1523,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>409.8730492362249</v>
+        <v>401.9897190108858</v>
       </c>
     </row>
     <row r="16">
@@ -1012,16 +1532,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C16">
-        <v>486.6780976954748</v>
+        <v>530.8101088838703</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1029,25 +1549,25 @@
         </is>
       </c>
       <c r="C17">
-        <v>512.7818692352064</v>
+        <v>411.3727121073692</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C18">
-        <v>489.6933609715219</v>
+        <v>557.4091168974911</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1055,25 +1575,25 @@
         </is>
       </c>
       <c r="C19">
-        <v>494.0761626838256</v>
+        <v>436.7841607835688</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C20">
-        <v>483.3777925090147</v>
+        <v>533.0470565860779</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1081,25 +1601,25 @@
         </is>
       </c>
       <c r="C21">
-        <v>472.1362615671298</v>
+        <v>418.5047966022299</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C22">
-        <v>424.526403628908</v>
+        <v>533.2516154902702</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1107,25 +1627,25 @@
         </is>
       </c>
       <c r="C23">
-        <v>438.5705964772461</v>
+        <v>429.7164467236912</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C24">
-        <v>471.3764140181302</v>
+        <v>517.8212343705832</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1133,20 +1653,163 @@
         </is>
       </c>
       <c r="C25">
-        <v>460.6123741655142</v>
+        <v>425.8828116573069</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
+        <v>2019</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>500.2558314571635</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2019</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>424.8558592138943</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2020</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>448.7839798504699</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2020</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>382.1038390653079</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2021</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>472.8160681242922</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>2021</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>384.1682453362131</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2022</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>507.9022331497652</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2022</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>409.5995288774203</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>2023</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>489.3818966207809</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2023</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Mujer</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>412.9400731529665</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
         <v>2024</v>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Hombre</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>466.7954394666047</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>2024</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Mujer</t>
         </is>
       </c>
-      <c r="C26">
-        <v>447.2688240083684</v>
+      <c r="C37">
+        <v>412.8568313195101</v>
       </c>
     </row>
   </sheetData>
@@ -1156,7 +1819,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1189,7 +1852,7 @@
         </is>
       </c>
       <c r="C2">
-        <v>635.751896585453</v>
+        <v>403.1541500747061</v>
       </c>
     </row>
     <row r="3">
@@ -1202,7 +1865,7 @@
         </is>
       </c>
       <c r="C3">
-        <v>306.4644513698159</v>
+        <v>252.2992029726032</v>
       </c>
     </row>
     <row r="4">
@@ -1215,7 +1878,7 @@
         </is>
       </c>
       <c r="C4">
-        <v>462.7588279084619</v>
+        <v>274.388606869013</v>
       </c>
     </row>
     <row r="5">
@@ -1228,7 +1891,7 @@
         </is>
       </c>
       <c r="C5">
-        <v>182.8369808098475</v>
+        <v>238.9905994789249</v>
       </c>
     </row>
     <row r="6">
@@ -1241,7 +1904,7 @@
         </is>
       </c>
       <c r="C6">
-        <v>650.4702380081842</v>
+        <v>416.1916908145654</v>
       </c>
     </row>
     <row r="7">
@@ -1254,7 +1917,7 @@
         </is>
       </c>
       <c r="C7">
-        <v>309.440018599861</v>
+        <v>257.475140683857</v>
       </c>
     </row>
     <row r="8">
@@ -1267,7 +1930,7 @@
         </is>
       </c>
       <c r="C8">
-        <v>459.0408988090194</v>
+        <v>289.9141468487847</v>
       </c>
     </row>
     <row r="9">
@@ -1280,7 +1943,7 @@
         </is>
       </c>
       <c r="C9">
-        <v>201.3799564968397</v>
+        <v>263.1287520398575</v>
       </c>
     </row>
     <row r="10">
@@ -1293,7 +1956,7 @@
         </is>
       </c>
       <c r="C10">
-        <v>644.3030200761755</v>
+        <v>390.9603738492736</v>
       </c>
     </row>
     <row r="11">
@@ -1306,7 +1969,7 @@
         </is>
       </c>
       <c r="C11">
-        <v>281.6863175991707</v>
+        <v>276.7883197848543</v>
       </c>
     </row>
     <row r="12">
@@ -1319,7 +1982,7 @@
         </is>
       </c>
       <c r="C12">
-        <v>459.0442445122263</v>
+        <v>277.8079595433991</v>
       </c>
     </row>
     <row r="13">
@@ -1332,7 +1995,7 @@
         </is>
       </c>
       <c r="C13">
-        <v>195.6486429108716</v>
+        <v>270.0118642272213</v>
       </c>
     </row>
     <row r="14">
@@ -1345,7 +2008,7 @@
         </is>
       </c>
       <c r="C14">
-        <v>679.5627435427527</v>
+        <v>439.5833814369253</v>
       </c>
     </row>
     <row r="15">
@@ -1358,7 +2021,7 @@
         </is>
       </c>
       <c r="C15">
-        <v>306.9906481113901</v>
+        <v>298.0777295174145</v>
       </c>
     </row>
     <row r="16">
@@ -1371,7 +2034,7 @@
         </is>
       </c>
       <c r="C16">
-        <v>498.2077867408416</v>
+        <v>336.4861420151558</v>
       </c>
     </row>
     <row r="17">
@@ -1384,7 +2047,7 @@
         </is>
       </c>
       <c r="C17">
-        <v>217.7012481661698</v>
+        <v>305.3774292708312</v>
       </c>
     </row>
     <row r="18">
@@ -1397,7 +2060,7 @@
         </is>
       </c>
       <c r="C18">
-        <v>649.4303368898422</v>
+        <v>456.2446230805709</v>
       </c>
     </row>
     <row r="19">
@@ -1410,7 +2073,7 @@
         </is>
       </c>
       <c r="C19">
-        <v>315.6591116859241</v>
+        <v>328.2640464730235</v>
       </c>
     </row>
     <row r="20">
@@ -1423,7 +2086,7 @@
         </is>
       </c>
       <c r="C20">
-        <v>519.7652885581499</v>
+        <v>345.9211285152657</v>
       </c>
     </row>
     <row r="21">
@@ -1436,7 +2099,7 @@
         </is>
       </c>
       <c r="C21">
-        <v>227.2432979442867</v>
+        <v>318.8949000167136</v>
       </c>
     </row>
     <row r="22">
@@ -1449,7 +2112,7 @@
         </is>
       </c>
       <c r="C22">
-        <v>661.3791187753011</v>
+        <v>478.3197905872174</v>
       </c>
     </row>
     <row r="23">
@@ -1462,7 +2125,7 @@
         </is>
       </c>
       <c r="C23">
-        <v>346.6338243686364</v>
+        <v>394.3376376677538</v>
       </c>
     </row>
     <row r="24">
@@ -1475,7 +2138,7 @@
         </is>
       </c>
       <c r="C24">
-        <v>572.8613961599586</v>
+        <v>392.6605696601817</v>
       </c>
     </row>
     <row r="25">
@@ -1488,7 +2151,7 @@
         </is>
       </c>
       <c r="C25">
-        <v>255.9427431104037</v>
+        <v>360.847227296584</v>
       </c>
     </row>
     <row r="26">
@@ -1501,7 +2164,7 @@
         </is>
       </c>
       <c r="C26">
-        <v>809.2125233037325</v>
+        <v>563.4437133012755</v>
       </c>
     </row>
     <row r="27">
@@ -1514,7 +2177,7 @@
         </is>
       </c>
       <c r="C27">
-        <v>354.29062105384</v>
+        <v>390.5697710055606</v>
       </c>
     </row>
     <row r="28">
@@ -1527,7 +2190,7 @@
         </is>
       </c>
       <c r="C28">
-        <v>603.8727660348862</v>
+        <v>417.5205148416082</v>
       </c>
     </row>
     <row r="29">
@@ -1540,7 +2203,7 @@
         </is>
       </c>
       <c r="C29">
-        <v>264.0524326207362</v>
+        <v>386.0485349183097</v>
       </c>
     </row>
     <row r="30">
@@ -1549,11 +2212,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C30">
-        <v>708.5945464495654</v>
+        <v>578.4775302755786</v>
       </c>
     </row>
     <row r="31">
@@ -1562,16 +2225,16 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Mujer Soltero/Otro</t>
+          <t>Hombre Soltero/Otro</t>
         </is>
       </c>
       <c r="C31">
-        <v>334.8982067701688</v>
+        <v>420.3282688668841</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1579,12 +2242,12 @@
         </is>
       </c>
       <c r="C32">
-        <v>751.8978538401648</v>
+        <v>433.9060688588612</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1592,38 +2255,38 @@
         </is>
       </c>
       <c r="C33">
-        <v>344.1202670192482</v>
+        <v>386.6347128975225</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C34">
-        <v>745.1114023301905</v>
+        <v>605.6846126685359</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Mujer Soltero/Otro</t>
+          <t>Hombre Soltero/Otro</t>
         </is>
       </c>
       <c r="C35">
-        <v>322.398088867876</v>
+        <v>440.1928132849202</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -1631,12 +2294,12 @@
         </is>
       </c>
       <c r="C36">
-        <v>740.1260548797701</v>
+        <v>449.3312771671951</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -1644,38 +2307,38 @@
         </is>
       </c>
       <c r="C37">
-        <v>341.6877065995374</v>
+        <v>421.9312038823365</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C38">
-        <v>749.1053433693304</v>
+        <v>579.6607206873761</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mujer Soltero/Otro</t>
+          <t>Hombre Soltero/Otro</t>
         </is>
       </c>
       <c r="C39">
-        <v>329.020887043152</v>
+        <v>417.933317199883</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -1683,12 +2346,12 @@
         </is>
       </c>
       <c r="C40">
-        <v>747.903250711925</v>
+        <v>435.8266128423639</v>
       </c>
     </row>
     <row r="41">
       <c r="A41">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1696,38 +2359,38 @@
         </is>
       </c>
       <c r="C41">
-        <v>318.5432701628077</v>
+        <v>397.6804652930945</v>
       </c>
     </row>
     <row r="42">
       <c r="A42">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C42">
-        <v>726.3949341739985</v>
+        <v>574.2386268936818</v>
       </c>
     </row>
     <row r="43">
       <c r="A43">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Mujer Soltero/Otro</t>
+          <t>Hombre Soltero/Otro</t>
         </is>
       </c>
       <c r="C43">
-        <v>289.4550943236467</v>
+        <v>435.4234572861184</v>
       </c>
     </row>
     <row r="44">
       <c r="A44">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1735,12 +2398,12 @@
         </is>
       </c>
       <c r="C44">
-        <v>750.7612366230678</v>
+        <v>435.1584693589547</v>
       </c>
     </row>
     <row r="45">
       <c r="A45">
-        <v>2021</v>
+        <v>2017</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1748,38 +2411,38 @@
         </is>
       </c>
       <c r="C45">
-        <v>294.9396205240269</v>
+        <v>423.2707831490498</v>
       </c>
     </row>
     <row r="46">
       <c r="A46">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C46">
-        <v>776.733687976842</v>
+        <v>561.7976445969257</v>
       </c>
     </row>
     <row r="47">
       <c r="A47">
-        <v>2022</v>
+        <v>2018</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Mujer Soltero/Otro</t>
+          <t>Hombre Soltero/Otro</t>
         </is>
       </c>
       <c r="C47">
-        <v>325.768860659345</v>
+        <v>425.1453899109132</v>
       </c>
     </row>
     <row r="48">
       <c r="A48">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1787,12 +2450,12 @@
         </is>
       </c>
       <c r="C48">
-        <v>734.661431099381</v>
+        <v>419.9153351695933</v>
       </c>
     </row>
     <row r="49">
       <c r="A49">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1800,33 +2463,319 @@
         </is>
       </c>
       <c r="C49">
-        <v>340.2854926740274</v>
+        <v>432.2557126148705</v>
       </c>
     </row>
     <row r="50">
       <c r="A50">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Mujer Casado/Unido</t>
+          <t>Hombre Casado/Unido</t>
         </is>
       </c>
       <c r="C50">
-        <v>753.0677600400326</v>
+        <v>540.5354145567755</v>
       </c>
     </row>
     <row r="51">
       <c r="A51">
+        <v>2019</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>414.1910777706792</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>2019</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>425.417541899797</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2019</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Mujer Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>424.2612639398942</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2020</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Hombre Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>492.926784289747</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>2020</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>358.1165475828636</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56">
+        <v>2020</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C56">
+        <v>438.0608497026322</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57">
+        <v>2020</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Mujer Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C57">
+        <v>332.2971395793116</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>2021</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Hombre Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C58">
+        <v>520.8911290727447</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>2021</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C59">
+        <v>377.9096475865106</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60">
+        <v>2021</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C60">
+        <v>402.6872218364642</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>2021</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Mujer Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C61">
+        <v>364.9576589062128</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>2022</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Hombre Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C62">
+        <v>556.9018328856565</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63">
+        <v>2022</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C63">
+        <v>416.1766767395839</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>2022</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C64">
+        <v>448.573333118281</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>2022</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Mujer Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C65">
+        <v>375.8877833117823</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>2023</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Hombre Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C66">
+        <v>526.3714138218139</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67">
+        <v>2023</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C67">
+        <v>424.4843475749711</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68">
+        <v>2023</v>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C68">
+        <v>445.8621977955382</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69">
+        <v>2023</v>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Mujer Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C69">
+        <v>384.9900868392327</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70">
         <v>2024</v>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Hombre Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C70">
+        <v>499.7371421400593</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71">
+        <v>2024</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Hombre Soltero/Otro</t>
+        </is>
+      </c>
+      <c r="C71">
+        <v>411.3344846142085</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72">
+        <v>2024</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>Mujer Casado/Unido</t>
+        </is>
+      </c>
+      <c r="C72">
+        <v>444.8687492647211</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73">
+        <v>2024</v>
+      </c>
+      <c r="B73" t="inlineStr">
         <is>
           <t>Mujer Soltero/Otro</t>
         </is>
       </c>
-      <c r="C51">
-        <v>321.3423482137987</v>
+      <c r="C73">
+        <v>385.9199417101463</v>
       </c>
     </row>
   </sheetData>
@@ -2334,7 +3283,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2357,6 +3306,708 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2">
+        <v>2007</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C2">
+        <v>371.6321398728473</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>2007</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C3">
+        <v>234.0551318402603</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>2007</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C4">
+        <v>240.3933229970801</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>2008</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C5">
+        <v>382.6568207741287</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>2008</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C6">
+        <v>272.8179393292757</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>2008</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C7">
+        <v>250.2284916270268</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>2009</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C8">
+        <v>367.6487952225102</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>2009</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C9">
+        <v>244.2941453714182</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>2009</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C10">
+        <v>258.5784982542586</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>2010</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C11">
+        <v>410.9964832394442</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>2010</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C12">
+        <v>272.4276630708343</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>2010</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C13">
+        <v>293.5217924968475</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>2011</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C14">
+        <v>427.5593172772525</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>2011</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C15">
+        <v>264.0844258599312</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <v>2011</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C16">
+        <v>319.735043272465</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>2012</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C17">
+        <v>465.4572707435492</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>2012</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C18">
+        <v>279.2620266752211</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>2012</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C19">
+        <v>367.9211301755064</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C20">
+        <v>518.6416996222624</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>2013</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C21">
+        <v>307.7701691197923</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>2013</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C22">
+        <v>393.5065763015224</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>2014</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C23">
+        <v>534.3478896161751</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>2014</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C24">
+        <v>304.534076462877</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>2014</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C25">
+        <v>414.1971361822961</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2015</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C26">
+        <v>568.8458232348481</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>2015</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C27">
+        <v>307.4473985743977</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>2015</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C28">
+        <v>421.6925767122177</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>2016</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C29">
+        <v>538.0230889811311</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>2016</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C30">
+        <v>296.5419257931907</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>2016</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C31">
+        <v>414.8068462546254</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>2017</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C32">
+        <v>544.4200242907084</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33">
+        <v>2017</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C33">
+        <v>284.2267508654468</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34">
+        <v>2017</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C34">
+        <v>419.8933818155351</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35">
+        <v>2018</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C35">
+        <v>529.2445978970717</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36">
+        <v>2018</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C36">
+        <v>301.4357715852863</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37">
+        <v>2018</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C37">
+        <v>412.2312612054813</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38">
+        <v>2019</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C38">
+        <v>517.7045351710772</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39">
+        <v>2019</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C39">
+        <v>291.6407038653007</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>2019</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C40">
+        <v>396.7685220333718</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>2020</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C41">
+        <v>463.3127945910567</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42">
+        <v>2020</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C42">
+        <v>276.773755940475</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>2020</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C43">
+        <v>357.4935928154939</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>2021</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C44">
+        <v>482.3467083338626</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45">
+        <v>2021</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C45">
+        <v>278.6039850534182</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>2021</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C46">
+        <v>368.5139185091243</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>2022</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C47">
+        <v>516.1706465123028</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>2022</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C48">
+        <v>310.8894507814023</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>2022</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C49">
+        <v>391.2270042539826</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>2023</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C50">
+        <v>510.1585770009571</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51">
+        <v>2023</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C51">
+        <v>290.9464103260765</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>2023</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C52">
+        <v>373.4642947690778</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>2024</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Adultos (30-64)</t>
+        </is>
+      </c>
+      <c r="C53">
+        <v>488.8292084382394</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54">
+        <v>2024</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Adultos mayores (65+)</t>
+        </is>
+      </c>
+      <c r="C54">
+        <v>291.6021592945477</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55">
+        <v>2024</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Jóvenes (18-29)</t>
+        </is>
+      </c>
+      <c r="C55">
+        <v>382.8949340713725</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>